<commit_message>
Fixed the issue with date formatting, and changed the statistic for TotalCreatedCampaignsCount.
</commit_message>
<xml_diff>
--- a/UnitedForUkraine.Server/Templates/ExcelTemplates/FoundationStatisticsTemplate.xlsx
+++ b/UnitedForUkraine.Server/Templates/ExcelTemplates/FoundationStatisticsTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CSharp-Projects\Web\UnitedForUkraine\UnitedForUkraine.Server\Templates\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FCBE54-EB70-4117-8496-0EAEE854E3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68135E82-789A-48A0-B019-82F6F8F52EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Indicator</t>
   </si>
@@ -75,20 +75,26 @@
     <t>Uniquer donors count</t>
   </si>
   <si>
-    <t>Active Campaigns count</t>
-  </si>
-  <si>
     <t>Created News updates count</t>
   </si>
   <si>
     <t>The best donor total donations count</t>
+  </si>
+  <si>
+    <t>Created Campaigns count</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="#,##0.00\ _₴"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,8 +126,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +154,11 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -159,11 +186,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,9 +202,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="40% - Accent2" xfId="1" builtinId="35"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,8 +528,8 @@
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
+      <c r="C5" s="5">
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -501,8 +539,8 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
+      <c r="C6" s="5">
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -512,8 +550,8 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
+      <c r="C7" s="5">
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -521,10 +559,10 @@
     </row>
     <row r="8" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
@@ -532,10 +570,10 @@
     </row>
     <row r="9" spans="2:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -545,10 +583,10 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -556,10 +594,10 @@
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -567,10 +605,10 @@
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -578,10 +616,10 @@
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -589,11 +627,11 @@
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -609,10 +647,10 @@
     </row>
     <row r="16" spans="2:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
@@ -623,5 +661,6 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added missing foundation statistics properties, added a list of related NewsUpdates on the CampaignDetailPage, and improved news update section styles.
</commit_message>
<xml_diff>
--- a/UnitedForUkraine.Server/Templates/ExcelTemplates/FoundationStatisticsTemplate.xlsx
+++ b/UnitedForUkraine.Server/Templates/ExcelTemplates/FoundationStatisticsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CSharp-Projects\Web\UnitedForUkraine\UnitedForUkraine.Server\Templates\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68135E82-789A-48A0-B019-82F6F8F52EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36B0273-BD9C-4362-BC62-EC926A4E6296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Count of registered users</t>
   </si>
   <si>
-    <t>Uniquer donors count</t>
-  </si>
-  <si>
     <t>Created News updates count</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Custom</t>
+  </si>
+  <si>
+    <t>Unique donors count</t>
   </si>
 </sst>
 </file>
@@ -92,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.00\ _₴"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ _₴"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -199,10 +199,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -210,6 +207,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,11 +507,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="4" spans="2:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -528,7 +528,7 @@
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -539,7 +539,7 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -548,9 +548,9 @@
     </row>
     <row r="7" spans="2:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="5">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -559,9 +559,9 @@
     </row>
     <row r="8" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -570,9 +570,9 @@
     </row>
     <row r="9" spans="2:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -583,10 +583,10 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -594,10 +594,10 @@
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -605,10 +605,10 @@
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -616,10 +616,10 @@
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -627,11 +627,11 @@
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>19</v>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -647,9 +647,9 @@
     </row>
     <row r="16" spans="2:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="5">
+        <v>16</v>
+      </c>
+      <c r="C16" s="4">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">

</xml_diff>

<commit_message>
Added finishing campaign feature when the goal amount is reached, improved the Report page structure, added GetCampaignsCountAsync and GetDonationsCountAsync methods, and added TotalAmountInUah statistics.
</commit_message>
<xml_diff>
--- a/UnitedForUkraine.Server/Templates/ExcelTemplates/FoundationStatisticsTemplate.xlsx
+++ b/UnitedForUkraine.Server/Templates/ExcelTemplates/FoundationStatisticsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CSharp-Projects\Web\UnitedForUkraine\UnitedForUkraine.Server\Templates\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36B0273-BD9C-4362-BC62-EC926A4E6296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C52E114-8429-4207-BDAE-4FBFAE1D9131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Indicator</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Created News updates count</t>
   </si>
   <si>
-    <t>The best donor total donations count</t>
-  </si>
-  <si>
     <t>Created Campaigns count</t>
   </si>
   <si>
@@ -85,6 +82,12 @@
   </si>
   <si>
     <t>Unique donors count</t>
+  </si>
+  <si>
+    <t>The best donor  donations count</t>
+  </si>
+  <si>
+    <t>The best donor total amount</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ _₴"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,8 +145,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +170,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -186,12 +202,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,9 +228,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="40% - Accent2" xfId="1" builtinId="35"/>
+    <cellStyle name="Accent6" xfId="3" builtinId="49"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -493,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +572,7 @@
     </row>
     <row r="7" spans="2:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
@@ -559,7 +583,7 @@
     </row>
     <row r="8" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
@@ -631,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -647,13 +671,24 @@
     </row>
     <row r="16" spans="2:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>